<commit_message>
link to about us,done
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -380,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +399,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2323</v>
+        <v>122232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2323</v>
+        <v>232323</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,7 +446,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>1077470550</v>
+        <v>10774750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>